<commit_message>
App update with nearly-complete quality checks on data up through October 1 2024
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/Variable_names.xlsx
+++ b/Microclimate_data_supporting/Variable_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{EACBFC19-F822-4CC4-82B9-DDB2F19CB23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D748BB4F-3484-415A-858A-52D7C4975E72}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{EACBFC19-F822-4CC4-82B9-DDB2F19CB23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B53C4A-A248-471C-9F29-3192D1BF7CFA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1C4F6A3-AE6D-4272-B375-FD5A72E2019B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>RHRelativeHumidity</t>
   </si>
@@ -303,13 +303,43 @@
   </si>
   <si>
     <t>mmhMaxPrecipRate_ExtraSensor</t>
+  </si>
+  <si>
+    <t>mmWaterContent</t>
+  </si>
+  <si>
+    <t>CTemperature</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>PYR</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>LWS</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A41</t>
+  </si>
+  <si>
+    <t>ECRN-100</t>
+  </si>
+  <si>
+    <t>Label.loc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +351,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,6 +400,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,21 +703,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDA614A-6119-4428-80C1-5E5B3BF92819}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -691,10 +733,16 @@
         <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -707,11 +755,17 @@
       <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2">
+        <v>-2</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -724,11 +778,17 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -741,11 +801,17 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -758,11 +824,17 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5">
+        <v>86.5</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -775,11 +847,17 @@
       <c r="D6" t="s">
         <v>66</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -792,11 +870,17 @@
       <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -809,11 +893,14 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -826,8 +913,14 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -840,11 +933,14 @@
       <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -857,11 +953,17 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -874,11 +976,17 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -891,8 +999,11 @@
       <c r="D13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -905,8 +1016,11 @@
       <c r="D14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -919,8 +1033,11 @@
       <c r="D15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -928,10 +1045,10 @@
         <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -939,10 +1056,10 @@
         <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -952,11 +1069,17 @@
       <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -969,8 +1092,11 @@
       <c r="D19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -983,8 +1109,11 @@
       <c r="D20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -997,11 +1126,17 @@
       <c r="D21" t="s">
         <v>58</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1014,8 +1149,11 @@
       <c r="D22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1026,7 +1164,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1034,7 +1172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -1042,7 +1180,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1050,7 +1188,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1058,7 +1196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1071,11 +1209,17 @@
       <c r="D28" t="s">
         <v>79</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1088,19 +1232,32 @@
       <c r="D29" t="s">
         <v>80</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30">
+        <v>440</v>
+      </c>
+      <c r="G30">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>